<commit_message>
Se añadieron cambios mostrados al jefe
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -764,7 +764,7 @@
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
@@ -931,8 +931,10 @@
       <c r="K3" t="n">
         <v>0</v>
       </c>
-      <c r="L3" t="n">
-        <v>0</v>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
       </c>
       <c r="M3" t="n">
         <v>0</v>

</xml_diff>